<commit_message>
Phinney study of performance on keto
</commit_message>
<xml_diff>
--- a/Studies/Ketogenic Diet/Energy Output/VO2max Testing/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04.xlsx
+++ b/Studies/Ketogenic Diet/Energy Output/VO2max Testing/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="615" windowWidth="18855" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="510" yWindow="675" windowWidth="18855" windowHeight="7560" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>time</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>%Fat</t>
+  </si>
+  <si>
+    <t>%Carbs</t>
+  </si>
+  <si>
+    <t>%VO2max</t>
   </si>
 </sst>
 </file>
@@ -198,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -356,6 +362,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -377,7 +454,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="1"/>
@@ -394,10 +471,61 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Accent" xfId="7"/>
@@ -1306,11 +1434,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115756416"/>
-        <c:axId val="115762304"/>
+        <c:axId val="85600128"/>
+        <c:axId val="85601664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115756416"/>
+        <c:axId val="85600128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,12 +1448,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115762304"/>
+        <c:crossAx val="85601664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115762304"/>
+        <c:axId val="85601664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,13 +1464,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115756416"/>
+        <c:crossAx val="85600128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1708,11 +1837,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115795456"/>
-        <c:axId val="115796992"/>
+        <c:axId val="85630976"/>
+        <c:axId val="85632512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115795456"/>
+        <c:axId val="85630976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -1725,12 +1854,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115796992"/>
+        <c:crossAx val="85632512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115796992"/>
+        <c:axId val="85632512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1743,7 +1872,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115795456"/>
+        <c:crossAx val="85630976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2085,11 +2214,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123227136"/>
-        <c:axId val="123228928"/>
+        <c:axId val="87001728"/>
+        <c:axId val="87007616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123227136"/>
+        <c:axId val="87001728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -2101,12 +2230,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123228928"/>
+        <c:crossAx val="87007616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123228928"/>
+        <c:axId val="87007616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2119,7 +2248,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123227136"/>
+        <c:crossAx val="87001728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2328,11 +2457,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123279232"/>
-        <c:axId val="123280768"/>
+        <c:axId val="89283584"/>
+        <c:axId val="89289472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123279232"/>
+        <c:axId val="89283584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -2345,12 +2474,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123280768"/>
+        <c:crossAx val="89289472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123280768"/>
+        <c:axId val="89289472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -2362,7 +2491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123279232"/>
+        <c:crossAx val="89283584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2488,11 +2617,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="127156608"/>
-        <c:axId val="125237888"/>
+        <c:axId val="89356160"/>
+        <c:axId val="89357696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127156608"/>
+        <c:axId val="89356160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2504,12 +2633,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125237888"/>
+        <c:crossAx val="89357696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125237888"/>
+        <c:axId val="89357696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2520,7 +2649,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127156608"/>
+        <c:crossAx val="89356160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2528,6 +2657,423 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Heart Rate vs %VO2Max</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1733888888888889"/>
+          <c:y val="4.1666666666666664E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>%VO2Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.8650164430708906E-3"/>
+                  <c:y val="0.50599462738390577"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                      <a:t>y = 0.0101x - 0.6486
+R² = 0.9676</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>0.12280701754385964</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0643274853801165E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10818713450292397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6491228070175419E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10526315789473684</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11695906432748537</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17251461988304093</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20760233918128651</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.17251461988304093</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22807017543859648</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22807017543859648</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.27777777777777773</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.27192982456140352</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.34795321637426901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.41812865497076024</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.40350877192982454</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.48538011695906436</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.48245614035087714</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.42690058479532161</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.49122807017543857</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.58771929824561397</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.62573099415204669</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.67836257309941517</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.62280701754385959</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.64912280701754377</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.76608187134502914</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.72514619883040932</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.78070175438596479</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.7192982456140351</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.85964912280701744</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.85964912280701744</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.86257309941520466</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.95614035087719296</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9385964912280701</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.97076023391812871</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="89602688"/>
+        <c:axId val="99017088"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="89602688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="170"/>
+          <c:min val="65"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99017088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="99017088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89602688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.41322977443819037"/>
+          <c:y val="0.78807464135476213"/>
+          <c:w val="0.18128909019794492"/>
+          <c:h val="7.8921621355056051E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2704,6 +3250,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3001,8 +3579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F36"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4148,7 +4726,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4780,18 +5358,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4921,7 +5500,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1"/>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1">
       <c r="A17" s="13" t="s">
         <v>3</v>
       </c>
@@ -4935,183 +5514,405 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" s="8">
         <v>120</v>
       </c>
       <c r="B18" s="5">
-        <f>((0.6681*A18)-9.9697)/100</f>
+        <f t="shared" ref="B18:B26" si="2">((0.6681*A18)-9.9697)/100</f>
         <v>0.70202299999999995</v>
       </c>
       <c r="C18" s="6">
-        <f>(-3.3333*B18)+3.3333</f>
+        <f t="shared" ref="C18:C27" si="3">(-3.3333*B18)+3.3333</f>
         <v>0.99324673409999997</v>
       </c>
       <c r="D18" s="9">
-        <f>1-C18</f>
+        <f t="shared" ref="D18:D27" si="4">1-C18</f>
         <v>6.7532659000000272E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" s="8">
         <v>125</v>
       </c>
       <c r="B19" s="5">
-        <f>((0.6681*A19)-9.9697)/100</f>
+        <f t="shared" si="2"/>
         <v>0.73542799999999997</v>
       </c>
       <c r="C19" s="6">
-        <f>(-3.3333*B19)+3.3333</f>
+        <f t="shared" si="3"/>
         <v>0.8818978475999999</v>
       </c>
       <c r="D19" s="9">
-        <f>1-C19</f>
+        <f t="shared" si="4"/>
         <v>0.1181021524000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" s="8">
         <v>130</v>
       </c>
       <c r="B20" s="5">
-        <f>((0.6681*A20)-9.9697)/100</f>
+        <f t="shared" si="2"/>
         <v>0.7688330000000001</v>
       </c>
       <c r="C20" s="6">
-        <f>(-3.3333*B20)+3.3333</f>
+        <f t="shared" si="3"/>
         <v>0.77054896109999982</v>
       </c>
       <c r="D20" s="9">
-        <f>1-C20</f>
+        <f t="shared" si="4"/>
         <v>0.22945103890000018</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" s="8">
         <v>135</v>
       </c>
       <c r="B21" s="5">
-        <f>((0.6681*A21)-9.9697)/100</f>
+        <f t="shared" si="2"/>
         <v>0.80223800000000001</v>
       </c>
       <c r="C21" s="6">
-        <f>(-3.3333*B21)+3.3333</f>
+        <f t="shared" si="3"/>
         <v>0.65920007460000019</v>
       </c>
       <c r="D21" s="9">
-        <f>1-C21</f>
+        <f t="shared" si="4"/>
         <v>0.34079992539999981</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" s="8">
         <v>140</v>
       </c>
       <c r="B22" s="5">
-        <f>((0.6681*A22)-9.9697)/100</f>
+        <f t="shared" si="2"/>
         <v>0.83564300000000002</v>
       </c>
       <c r="C22" s="6">
-        <f>(-3.3333*B22)+3.3333</f>
+        <f t="shared" si="3"/>
         <v>0.54785118810000011</v>
       </c>
       <c r="D22" s="9">
-        <f>1-C22</f>
+        <f t="shared" si="4"/>
         <v>0.45214881189999989</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" s="8">
         <v>145</v>
       </c>
       <c r="B23" s="5">
-        <f>((0.6681*A23)-9.9697)/100</f>
+        <f t="shared" si="2"/>
         <v>0.86904799999999993</v>
       </c>
       <c r="C23" s="6">
-        <f>(-3.3333*B23)+3.3333</f>
+        <f t="shared" si="3"/>
         <v>0.43650230160000003</v>
       </c>
       <c r="D23" s="9">
-        <f>1-C23</f>
+        <f t="shared" si="4"/>
         <v>0.56349769839999997</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" s="8">
         <v>150</v>
       </c>
       <c r="B24" s="5">
-        <f>((0.6681*A24)-9.9697)/100</f>
+        <f t="shared" si="2"/>
         <v>0.90245299999999995</v>
       </c>
       <c r="C24" s="6">
-        <f>(-3.3333*B24)+3.3333</f>
+        <f t="shared" si="3"/>
         <v>0.32515341509999995</v>
       </c>
       <c r="D24" s="9">
-        <f>1-C24</f>
+        <f t="shared" si="4"/>
         <v>0.67484658490000005</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" s="8">
         <v>155</v>
       </c>
       <c r="B25" s="5">
-        <f>((0.6681*A25)-9.9697)/100</f>
+        <f t="shared" si="2"/>
         <v>0.93585800000000008</v>
       </c>
       <c r="C25" s="6">
-        <f>(-3.3333*B25)+3.3333</f>
+        <f t="shared" si="3"/>
         <v>0.21380452859999988</v>
       </c>
       <c r="D25" s="9">
-        <f>1-C25</f>
+        <f t="shared" si="4"/>
         <v>0.78619547140000012</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="8">
         <v>160</v>
       </c>
       <c r="B26" s="5">
-        <f>((0.6681*A26)-9.9697)/100</f>
+        <f t="shared" si="2"/>
         <v>0.96926299999999999</v>
       </c>
       <c r="C26" s="6">
-        <f>(-3.3333*B26)+3.3333</f>
+        <f t="shared" si="3"/>
         <v>0.10245564210000024</v>
       </c>
       <c r="D26" s="9">
-        <f>1-C26</f>
+        <f t="shared" si="4"/>
         <v>0.89754435789999976</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1">
+    <row r="27" spans="1:5" ht="15" thickBot="1">
       <c r="A27" s="10">
         <v>165</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="16">
         <v>1</v>
       </c>
       <c r="C27" s="11">
-        <f>(-3.3333*B27)+3.3333</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D27" s="12">
-        <f>1-C27</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18"/>
+    <row r="31" spans="1:5" ht="15" thickBot="1"/>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A32" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="29">
+        <v>120</v>
+      </c>
+      <c r="B33" s="30">
+        <f t="shared" ref="B33:B41" si="5">((0.6681*A33)-9.9697)/100</f>
+        <v>0.70202299999999995</v>
+      </c>
+      <c r="C33" s="31">
+        <f t="shared" ref="C33:C42" si="6">(-3.3333*B33)+3.3333</f>
+        <v>0.99324673409999997</v>
+      </c>
+      <c r="D33" s="32">
+        <f t="shared" ref="D33:D42" si="7">1-C33</f>
+        <v>6.7532659000000272E-3</v>
+      </c>
+      <c r="E33" s="33">
+        <f>(0.0101*A33)-0.6486</f>
+        <v>0.56340000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="20">
+        <v>125</v>
+      </c>
+      <c r="B34" s="21">
+        <f t="shared" si="5"/>
+        <v>0.73542799999999997</v>
+      </c>
+      <c r="C34" s="22">
+        <f t="shared" si="6"/>
+        <v>0.8818978475999999</v>
+      </c>
+      <c r="D34" s="23">
+        <f t="shared" si="7"/>
+        <v>0.1181021524000001</v>
+      </c>
+      <c r="E34" s="28">
+        <f t="shared" ref="E34:E42" si="8">(0.0101*A34)-0.6486</f>
+        <v>0.6139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="20">
+        <v>130</v>
+      </c>
+      <c r="B35" s="21">
+        <f t="shared" si="5"/>
+        <v>0.7688330000000001</v>
+      </c>
+      <c r="C35" s="22">
+        <f t="shared" si="6"/>
+        <v>0.77054896109999982</v>
+      </c>
+      <c r="D35" s="23">
+        <f t="shared" si="7"/>
+        <v>0.22945103890000018</v>
+      </c>
+      <c r="E35" s="28">
+        <f t="shared" si="8"/>
+        <v>0.66439999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="20">
+        <v>135</v>
+      </c>
+      <c r="B36" s="21">
+        <f t="shared" si="5"/>
+        <v>0.80223800000000001</v>
+      </c>
+      <c r="C36" s="22">
+        <f t="shared" si="6"/>
+        <v>0.65920007460000019</v>
+      </c>
+      <c r="D36" s="23">
+        <f t="shared" si="7"/>
+        <v>0.34079992539999981</v>
+      </c>
+      <c r="E36" s="28">
+        <f t="shared" si="8"/>
+        <v>0.71489999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="20">
+        <v>140</v>
+      </c>
+      <c r="B37" s="21">
+        <f t="shared" si="5"/>
+        <v>0.83564300000000002</v>
+      </c>
+      <c r="C37" s="22">
+        <f t="shared" si="6"/>
+        <v>0.54785118810000011</v>
+      </c>
+      <c r="D37" s="23">
+        <f t="shared" si="7"/>
+        <v>0.45214881189999989</v>
+      </c>
+      <c r="E37" s="28">
+        <f t="shared" si="8"/>
+        <v>0.76539999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="20">
+        <v>145</v>
+      </c>
+      <c r="B38" s="21">
+        <f t="shared" si="5"/>
+        <v>0.86904799999999993</v>
+      </c>
+      <c r="C38" s="22">
+        <f t="shared" si="6"/>
+        <v>0.43650230160000003</v>
+      </c>
+      <c r="D38" s="23">
+        <f t="shared" si="7"/>
+        <v>0.56349769839999997</v>
+      </c>
+      <c r="E38" s="28">
+        <f t="shared" si="8"/>
+        <v>0.81589999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="20">
+        <v>150</v>
+      </c>
+      <c r="B39" s="21">
+        <f t="shared" si="5"/>
+        <v>0.90245299999999995</v>
+      </c>
+      <c r="C39" s="22">
+        <f t="shared" si="6"/>
+        <v>0.32515341509999995</v>
+      </c>
+      <c r="D39" s="23">
+        <f t="shared" si="7"/>
+        <v>0.67484658490000005</v>
+      </c>
+      <c r="E39" s="28">
+        <f t="shared" si="8"/>
+        <v>0.86639999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="20">
+        <v>155</v>
+      </c>
+      <c r="B40" s="21">
+        <f t="shared" si="5"/>
+        <v>0.93585800000000008</v>
+      </c>
+      <c r="C40" s="22">
+        <f t="shared" si="6"/>
+        <v>0.21380452859999988</v>
+      </c>
+      <c r="D40" s="23">
+        <f t="shared" si="7"/>
+        <v>0.78619547140000012</v>
+      </c>
+      <c r="E40" s="28">
+        <f t="shared" si="8"/>
+        <v>0.91689999999999994</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="20">
+        <v>160</v>
+      </c>
+      <c r="B41" s="21">
+        <f t="shared" si="5"/>
+        <v>0.96926299999999999</v>
+      </c>
+      <c r="C41" s="22">
+        <f t="shared" si="6"/>
+        <v>0.10245564210000024</v>
+      </c>
+      <c r="D41" s="23">
+        <f t="shared" si="7"/>
+        <v>0.89754435789999976</v>
+      </c>
+      <c r="E41" s="28">
+        <f t="shared" si="8"/>
+        <v>0.96739999999999993</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" thickBot="1">
+      <c r="A42" s="24">
+        <v>165</v>
+      </c>
+      <c r="B42" s="25">
+        <v>1</v>
+      </c>
+      <c r="C42" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D42" s="27">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="34">
+        <f t="shared" si="8"/>
+        <v>1.0179</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More studies more of my own VO2max data
</commit_message>
<xml_diff>
--- a/Studies/Ketogenic Diet/Energy Output/VO2max Testing/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04.xlsx
+++ b/Studies/Ketogenic Diet/Energy Output/VO2max Testing/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="675" windowWidth="18855" windowHeight="7560" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="510" yWindow="675" windowWidth="18855" windowHeight="7560" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="RER_HR" sheetId="6" r:id="rId2"/>
     <sheet name="RER_HR_Cut" sheetId="7" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId4"/>
+    <sheet name="PercentVO2_RER" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -454,7 +455,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="1"/>
@@ -526,6 +527,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Accent" xfId="7"/>
@@ -1434,11 +1436,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85600128"/>
-        <c:axId val="85601664"/>
+        <c:axId val="178399104"/>
+        <c:axId val="178400640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85600128"/>
+        <c:axId val="178399104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,12 +1450,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85601664"/>
+        <c:crossAx val="178400640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85601664"/>
+        <c:axId val="178400640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,7 +1466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85600128"/>
+        <c:crossAx val="178399104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1711,7 +1713,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$2:$E$38</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>0.12280701754385964</c:v>
@@ -1837,11 +1839,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85630976"/>
-        <c:axId val="85632512"/>
+        <c:axId val="131018752"/>
+        <c:axId val="131020288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85630976"/>
+        <c:axId val="131018752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -1854,12 +1856,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85632512"/>
+        <c:crossAx val="131020288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85632512"/>
+        <c:axId val="131020288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1868,11 +1870,11 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85630976"/>
+        <c:crossAx val="131018752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1933,7 +1935,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2214,11 +2215,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87001728"/>
-        <c:axId val="87007616"/>
+        <c:axId val="131033728"/>
+        <c:axId val="131035520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87001728"/>
+        <c:axId val="131033728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -2230,12 +2231,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87007616"/>
+        <c:crossAx val="131035520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87007616"/>
+        <c:axId val="131035520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2248,7 +2249,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87001728"/>
+        <c:crossAx val="131033728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2309,7 +2310,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2457,11 +2457,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="89283584"/>
-        <c:axId val="89289472"/>
+        <c:axId val="131232896"/>
+        <c:axId val="131234432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89283584"/>
+        <c:axId val="131232896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -2474,12 +2474,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89289472"/>
+        <c:crossAx val="131234432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89289472"/>
+        <c:axId val="131234432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -2491,7 +2491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89283584"/>
+        <c:crossAx val="131232896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2617,11 +2617,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="89356160"/>
-        <c:axId val="89357696"/>
+        <c:axId val="131006464"/>
+        <c:axId val="131008000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89356160"/>
+        <c:axId val="131006464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2633,12 +2633,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89357696"/>
+        <c:crossAx val="131008000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89357696"/>
+        <c:axId val="131008000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2649,7 +2649,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89356160"/>
+        <c:crossAx val="131006464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2896,7 +2896,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$2:$E$38</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>0.12280701754385964</c:v>
@@ -3022,11 +3022,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="89602688"/>
-        <c:axId val="99017088"/>
+        <c:axId val="131246336"/>
+        <c:axId val="131248128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89602688"/>
+        <c:axId val="131246336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -3039,12 +3039,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99017088"/>
+        <c:crossAx val="131248128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99017088"/>
+        <c:axId val="131248128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3053,11 +3053,11 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89602688"/>
+        <c:crossAx val="131246336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3088,20 +3088,465 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>%VO2max(x)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RER(y)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20947222222222223"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RER</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.7202973111896543E-2"/>
+                  <c:y val="-0.1306747757276609"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                      <a:t>y = -1.2618x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="30000"/>
+                      <a:t>3</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                      <a:t> + 3.2658x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                      <a:t> - 1.8989x + 0.9264
+R² = </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+                      <a:t>0.9519</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>0.12280701754385964</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0643274853801165E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10818713450292397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6491228070175419E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10526315789473684</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11695906432748537</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17251461988304093</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20760233918128651</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.17251461988304093</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22807017543859648</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22807017543859648</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.27777777777777773</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.27192982456140352</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.34795321637426901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.41812865497076024</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.40350877192982454</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.48538011695906436</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.48245614035087714</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.42690058479532161</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.49122807017543857</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.58771929824561397</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.62573099415204669</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.67836257309941517</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.62280701754385959</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.64912280701754377</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.76608187134502914</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.72514619883040932</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.78070175438596479</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.7192982456140351</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.85964912280701744</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.85964912280701744</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.86257309941520466</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.95614035087719296</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9385964912280701</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.97076023391812871</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="178412160"/>
+        <c:axId val="133501312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="178412160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="133501312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="133501312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.2"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="178412160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17541601049868771"/>
+          <c:y val="0.42316929133858266"/>
+          <c:w val="0.17065334770761972"/>
+          <c:h val="8.9964743213068521E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>42861</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>471486</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3122,16 +3567,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3282,6 +3727,43 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3579,8 +4061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3631,7 +4113,7 @@
       <c r="D2">
         <v>78</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="35">
         <f>$B2/$B$44</f>
         <v>0.12280701754385964</v>
       </c>
@@ -3657,7 +4139,7 @@
       <c r="D3">
         <v>78</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="35">
         <f t="shared" ref="E3:E42" si="2">$B3/$B$44</f>
         <v>9.0643274853801165E-2</v>
       </c>
@@ -3683,7 +4165,7 @@
       <c r="D4">
         <v>70</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="35">
         <f t="shared" si="2"/>
         <v>0.10818713450292397</v>
       </c>
@@ -3709,7 +4191,7 @@
       <c r="D5">
         <v>80</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="35">
         <f t="shared" si="2"/>
         <v>9.6491228070175419E-2</v>
       </c>
@@ -3735,7 +4217,7 @@
       <c r="D6">
         <v>84</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="35">
         <f t="shared" si="2"/>
         <v>0.10526315789473684</v>
       </c>
@@ -3761,7 +4243,7 @@
       <c r="D7">
         <v>76</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="35">
         <f t="shared" si="2"/>
         <v>0.11695906432748537</v>
       </c>
@@ -3787,7 +4269,7 @@
       <c r="D8">
         <v>84</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="35">
         <f t="shared" si="2"/>
         <v>0.17251461988304093</v>
       </c>
@@ -3813,7 +4295,7 @@
       <c r="D9">
         <v>92</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="35">
         <f t="shared" si="2"/>
         <v>0.20760233918128651</v>
       </c>
@@ -3839,7 +4321,7 @@
       <c r="D10">
         <v>84</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="35">
         <f t="shared" si="2"/>
         <v>0.16666666666666666</v>
       </c>
@@ -3865,7 +4347,7 @@
       <c r="D11">
         <v>82</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="35">
         <f t="shared" si="2"/>
         <v>0.17251461988304093</v>
       </c>
@@ -3891,7 +4373,7 @@
       <c r="D12">
         <v>88</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="35">
         <f t="shared" si="2"/>
         <v>0.22807017543859648</v>
       </c>
@@ -3917,7 +4399,7 @@
       <c r="D13">
         <v>88</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="35">
         <f t="shared" si="2"/>
         <v>0.22807017543859648</v>
       </c>
@@ -3943,7 +4425,7 @@
       <c r="D14">
         <v>90</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="35">
         <f t="shared" si="2"/>
         <v>0.27777777777777773</v>
       </c>
@@ -3969,7 +4451,7 @@
       <c r="D15">
         <v>94</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="35">
         <f t="shared" si="2"/>
         <v>0.27192982456140352</v>
       </c>
@@ -3995,7 +4477,7 @@
       <c r="D16">
         <v>97</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="35">
         <f t="shared" si="2"/>
         <v>0.34795321637426901</v>
       </c>
@@ -4021,7 +4503,7 @@
       <c r="D17">
         <v>99</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="35">
         <f t="shared" si="2"/>
         <v>0.41812865497076024</v>
       </c>
@@ -4047,7 +4529,7 @@
       <c r="D18">
         <v>102</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="35">
         <f t="shared" si="2"/>
         <v>0.40350877192982454</v>
       </c>
@@ -4073,7 +4555,7 @@
       <c r="D19">
         <v>103</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="35">
         <f t="shared" si="2"/>
         <v>0.48538011695906436</v>
       </c>
@@ -4099,7 +4581,7 @@
       <c r="D20">
         <v>106</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="35">
         <f t="shared" si="2"/>
         <v>0.48245614035087714</v>
       </c>
@@ -4125,7 +4607,7 @@
       <c r="D21">
         <v>114</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="35">
         <f t="shared" si="2"/>
         <v>0.42690058479532161</v>
       </c>
@@ -4151,7 +4633,7 @@
       <c r="D22">
         <v>106</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="35">
         <f t="shared" si="2"/>
         <v>0.49122807017543857</v>
       </c>
@@ -4177,7 +4659,7 @@
       <c r="D23">
         <v>109</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="35">
         <f t="shared" si="2"/>
         <v>0.58771929824561397</v>
       </c>
@@ -4203,7 +4685,7 @@
       <c r="D24">
         <v>117</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="35">
         <f t="shared" si="2"/>
         <v>0.62573099415204669</v>
       </c>
@@ -4229,7 +4711,7 @@
       <c r="D25">
         <v>124</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="35">
         <f t="shared" si="2"/>
         <v>0.67836257309941517</v>
       </c>
@@ -4255,7 +4737,7 @@
       <c r="D26">
         <v>126</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="35">
         <f t="shared" si="2"/>
         <v>0.62280701754385959</v>
       </c>
@@ -4281,7 +4763,7 @@
       <c r="D27">
         <v>129</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="35">
         <f t="shared" si="2"/>
         <v>0.64912280701754377</v>
       </c>
@@ -4307,7 +4789,7 @@
       <c r="D28">
         <v>135</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="35">
         <f t="shared" si="2"/>
         <v>0.76608187134502914</v>
       </c>
@@ -4333,7 +4815,7 @@
       <c r="D29">
         <v>138</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="35">
         <f t="shared" si="2"/>
         <v>0.72514619883040932</v>
       </c>
@@ -4359,7 +4841,7 @@
       <c r="D30">
         <v>138</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="35">
         <f t="shared" si="2"/>
         <v>0.78070175438596479</v>
       </c>
@@ -4385,7 +4867,7 @@
       <c r="D31">
         <v>139</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="35">
         <f t="shared" si="2"/>
         <v>0.7192982456140351</v>
       </c>
@@ -4411,7 +4893,7 @@
       <c r="D32">
         <v>143</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="35">
         <f t="shared" si="2"/>
         <v>0.85964912280701744</v>
       </c>
@@ -4437,7 +4919,7 @@
       <c r="D33">
         <v>149</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="35">
         <f t="shared" si="2"/>
         <v>0.85964912280701744</v>
       </c>
@@ -4463,7 +4945,7 @@
       <c r="D34">
         <v>155</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="35">
         <f t="shared" si="2"/>
         <v>0.86257309941520466</v>
       </c>
@@ -4489,7 +4971,7 @@
       <c r="D35">
         <v>158</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="35">
         <f t="shared" si="2"/>
         <v>0.95614035087719296</v>
       </c>
@@ -4515,7 +4997,7 @@
       <c r="D36">
         <v>161</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="35">
         <f t="shared" si="2"/>
         <v>0.9385964912280701</v>
       </c>
@@ -4541,7 +5023,7 @@
       <c r="D37">
         <v>165</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="35">
         <f t="shared" si="2"/>
         <v>0.97076023391812871</v>
       </c>
@@ -4570,7 +5052,7 @@
       <c r="D38">
         <v>167</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -4599,7 +5081,7 @@
       <c r="D39">
         <v>169</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="35">
         <f t="shared" si="2"/>
         <v>0.98830409356725135</v>
       </c>
@@ -4625,7 +5107,7 @@
       <c r="D40">
         <v>173</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="35">
         <f t="shared" si="2"/>
         <v>0.8157894736842104</v>
       </c>
@@ -4654,7 +5136,7 @@
       <c r="D41">
         <v>170</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="35">
         <f t="shared" si="2"/>
         <v>0.92690058479532156</v>
       </c>
@@ -4680,7 +5162,7 @@
       <c r="D42">
         <v>161</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="35">
         <f t="shared" si="2"/>
         <v>0.29532163742690054</v>
       </c>
@@ -5360,7 +5842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -5915,4 +6397,19 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>